<commit_message>
Added and Excel example
</commit_message>
<xml_diff>
--- a/examples.xlsx
+++ b/examples.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="360" windowWidth="11235" windowHeight="3885" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="360" windowWidth="11235" windowHeight="3885" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
     <sheet name="Grades" sheetId="3" r:id="rId2"/>
     <sheet name="Fruits" sheetId="2" r:id="rId3"/>
     <sheet name="Clients" sheetId="4" r:id="rId4"/>
+    <sheet name="Grades2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
   <si>
     <t>Students Database</t>
   </si>
@@ -191,6 +192,9 @@
   </si>
   <si>
     <t>Vehicles</t>
+  </si>
+  <si>
+    <t>Grades</t>
   </si>
 </sst>
 </file>
@@ -320,7 +324,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -612,7 +616,7 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -930,7 +934,7 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
@@ -1036,7 +1040,7 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1149,11 +1153,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -1519,4 +1523,89 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>